<commit_message>
mod u net corrected 30/100
</commit_message>
<xml_diff>
--- a/modified_u_net512x512.xlsx
+++ b/modified_u_net512x512.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,20 +441,30 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>binary_io_u</t>
+          <t>binary_io_u_3</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>dice_metric</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>val_loss</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>val_binary_io_u</t>
+          <t>val_binary_io_u_3</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>val_dice_metric</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>epoch</t>
         </is>
@@ -462,121 +472,439 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.236003875732422</v>
+        <v>1.065317153930664</v>
       </c>
       <c r="B2" t="n">
-        <v>0.38727205991745</v>
+        <v>0.4640493988990784</v>
       </c>
       <c r="C2" t="n">
-        <v>1.346005916595459</v>
+        <v>0.3548171520233154</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4916933178901672</v>
+        <v>1.271228075027466</v>
       </c>
       <c r="E2" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.2631695866584778</v>
+      </c>
+      <c r="G2" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.167133569717407</v>
+        <v>0.8141606450080872</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3988186120986938</v>
+        <v>0.5656570196151733</v>
       </c>
       <c r="C3" t="n">
-        <v>1.314587116241455</v>
+        <v>0.4668542444705963</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4561311006546021</v>
+        <v>1.176835894584656</v>
       </c>
       <c r="E3" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.2735696732997894</v>
+      </c>
+      <c r="G3" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.114528894424438</v>
+        <v>0.6438578963279724</v>
       </c>
       <c r="B4" t="n">
-        <v>0.42709881067276</v>
+        <v>0.6217673420906067</v>
       </c>
       <c r="C4" t="n">
-        <v>1.284281015396118</v>
+        <v>0.5723934769630432</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4569307267665863</v>
+        <v>1.089979887008667</v>
       </c>
       <c r="E4" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.2712994515895844</v>
+      </c>
+      <c r="G4" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1.0727299451828</v>
+        <v>0.4910151362419128</v>
       </c>
       <c r="B5" t="n">
-        <v>0.4542855024337769</v>
+        <v>0.6713499426841736</v>
       </c>
       <c r="C5" t="n">
-        <v>1.257749795913696</v>
+        <v>0.6832207441329956</v>
       </c>
       <c r="D5" t="n">
-        <v>0.4571948051452637</v>
+        <v>1.056345224380493</v>
       </c>
       <c r="E5" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.24927918612957</v>
+      </c>
+      <c r="G5" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1.033577084541321</v>
+        <v>0.4103506505489349</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4758060276508331</v>
+        <v>0.6957248449325562</v>
       </c>
       <c r="C6" t="n">
-        <v>1.230779409408569</v>
+        <v>0.7400398254394531</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4573077261447906</v>
+        <v>1.055898308753967</v>
       </c>
       <c r="E6" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.2041231691837311</v>
+      </c>
+      <c r="G6" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1.001506090164185</v>
+        <v>0.3730241358280182</v>
       </c>
       <c r="B7" t="n">
-        <v>0.4942916035652161</v>
+        <v>0.7027483582496643</v>
       </c>
       <c r="C7" t="n">
-        <v>1.204034805297852</v>
+        <v>0.7659919857978821</v>
       </c>
       <c r="D7" t="n">
-        <v>0.457369327545166</v>
+        <v>1.081430196762085</v>
       </c>
       <c r="E7" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.1559834629297256</v>
+      </c>
+      <c r="G7" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.9690195322036743</v>
+        <v>0.3533163666725159</v>
       </c>
       <c r="B8" t="n">
-        <v>0.5084222555160522</v>
+        <v>0.7108031511306763</v>
       </c>
       <c r="C8" t="n">
-        <v>1.178504824638367</v>
+        <v>0.7779204845428467</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4573939442634583</v>
+        <v>1.115687012672424</v>
       </c>
       <c r="E8" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.1152432933449745</v>
+      </c>
+      <c r="G8" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>0.3328442871570587</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.7127156853675842</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.7922288179397583</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.163525700569153</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.07983924448490143</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0.3264735341072083</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.7162885665893555</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.7952737808227539</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.191913723945618</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.06144086644053459</v>
+      </c>
+      <c r="G10" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0.3187452554702759</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.7206717729568481</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.7989698648452759</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.229954123497009</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.04168339446187019</v>
+      </c>
+      <c r="G11" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0.3118893504142761</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.7166717052459717</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.8046832084655762</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.257521867752075</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.03299479931592941</v>
+      </c>
+      <c r="G12" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0.3074690699577332</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.7213510274887085</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.8062549829483032</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.289356708526611</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.02305548079311848</v>
+      </c>
+      <c r="G13" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0.3030803203582764</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.7233078479766846</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.8082906603813171</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.319879174232483</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.01624204032123089</v>
+      </c>
+      <c r="G14" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>0.3050404191017151</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.7186112403869629</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.8076108694076538</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1.3380286693573</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.01414340455085039</v>
+      </c>
+      <c r="G15" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>0.2937130630016327</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.7252293825149536</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.8148374557495117</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.343879342079163</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.01307932287454605</v>
+      </c>
+      <c r="G16" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>0.2910315692424774</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.7261908054351807</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.8162949681282043</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1.366653919219971</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.01036407984793186</v>
+      </c>
+      <c r="G17" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>0.29124516248703</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.7235106825828552</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.8162726163864136</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.386469602584839</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.008140009827911854</v>
+      </c>
+      <c r="G18" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>0.2891172766685486</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.7251983880996704</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.8174265027046204</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.392734289169312</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.4574995040893555</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.007918978109955788</v>
+      </c>
+      <c r="G19" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>0.2851462960243225</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.727731466293335</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.8196375966072083</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.386369943618774</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.457520067691803</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.008769180625677109</v>
+      </c>
+      <c r="G20" t="n">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>